<commit_message>
cambio formato datos de entrada (nueva columna con tipo de commodity)
</commit_message>
<xml_diff>
--- a/data/dia_1.xlsx
+++ b/data/dia_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFG\flexible-vrp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vrp_basic_mip\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2704D63F-7129-40A5-BFB0-16EA3F99D994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913EF517-D900-4FAD-B186-8E8346BD34EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="52">
   <si>
     <t>name</t>
   </si>
@@ -119,6 +119,78 @@
   </si>
   <si>
     <t>no_stops</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>no_req_total</t>
+  </si>
+  <si>
+    <t>no_opt_total</t>
   </si>
 </sst>
 </file>
@@ -158,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,18 +614,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -569,7 +641,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -577,7 +649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -585,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -593,7 +665,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -601,7 +673,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -609,7 +681,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -617,7 +689,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -625,7 +697,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -633,7 +705,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -642,12 +714,30 @@
         <v>17.857142857142858</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <f>SUM(comp_quantity_inst1!C2:C12)</f>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14">
+        <f>SUM(comp_quantity_inst1!C13:C23)</f>
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -660,16 +750,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -680,7 +770,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -691,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -702,7 +792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -713,7 +803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -724,7 +814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -735,7 +825,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -746,7 +836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -757,7 +847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -768,7 +858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -779,7 +869,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -790,7 +880,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -801,7 +891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -812,7 +902,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -823,7 +913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -834,7 +924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -845,7 +935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -856,7 +946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -867,7 +957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -878,7 +968,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -889,7 +979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -900,7 +990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -911,7 +1001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -922,7 +1012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -933,7 +1023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -944,7 +1034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -955,7 +1045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -966,7 +1056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -977,7 +1067,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -988,7 +1078,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -999,7 +1089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -1010,7 +1100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1032,7 +1122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1133,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1054,7 +1144,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1065,7 +1155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1076,7 +1166,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1087,7 +1177,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1098,7 +1188,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1109,7 +1199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1120,7 +1210,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -1131,7 +1221,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1142,7 +1232,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1153,7 +1243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1164,7 +1254,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1175,7 +1265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1186,7 +1276,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1197,7 +1287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1208,7 +1298,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1219,7 +1309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -1230,7 +1320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -1241,7 +1331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1252,7 +1342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -1263,7 +1353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -1274,7 +1364,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -1285,7 +1375,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -1304,16 +1394,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1322,316 +1412,385 @@
       <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>11</v>
-      </c>
-      <c r="D2">
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
         <v>37</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
         <v>48</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
         <v>143</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10">
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
         <v>28</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>11</v>
-      </c>
-      <c r="D11">
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>51</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
-        <v>18</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
         <v>102</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E14" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
         <v>105</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2">
         <v>60</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E16" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2">
         <v>58</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E17" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>91</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E18" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2">
         <v>20</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20">
+      <c r="E19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2">
         <v>20</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="E20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>34</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22">
+      <c r="E21" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="2">
         <v>61</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="E22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>